<commit_message>
excel update. A mistake of shooter in xml is fixed
</commit_message>
<xml_diff>
--- a/BlockTileSystem/Assets/Levels/map_schema.xlsx
+++ b/BlockTileSystem/Assets/Levels/map_schema.xlsx
@@ -177,14 +177,17 @@
   <connection id="7" name="map3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\U3D\0.PROJECTS\BlockTileSystem\BlockTileSystem\BlockTileSystem\Assets\Levels\map.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="8" name="xml" type="4" refreshedVersion="0" background="1">
+  <connection id="8" name="map4" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="D:\U3D\0.PROJECTS\BlockTileSystem\BlockTileSystem\BlockTileSystem\Assets\Levels\map.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="9" name="xml" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\U3D\0.PROJECTS\BlockTileSystem\BlockTileSystem\BlockTileSystem\Assets\Levels\xml\xml.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -473,7 +476,7 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema4">
+  <Schema ID="Schema2">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="SavableLevel">
         <xsd:complexType>
@@ -588,7 +591,7 @@
                 </xsd:sequence>
               </xsd:complexType>
             </xsd:element>
-            <xsd:element minOccurs="0" nillable="true" name="Shooters" form="unqualified">
+            <xsd:element minOccurs="0" nillable="true" name="sShooters" form="unqualified">
               <xsd:complexType>
                 <xsd:sequence minOccurs="0">
                   <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="ShooterInXML" form="unqualified">
@@ -599,15 +602,15 @@
                             <xsd:sequence minOccurs="0">
                               <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="x" form="unqualified"/>
                               <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="y" form="unqualified"/>
-                              <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="shootingTimeInterval" form="unqualified"/>
-                              <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="sShootingDirection" form="unqualified"/>
-                              <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="isMoving" form="unqualified"/>
-                              <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="sMovingDirection" form="unqualified"/>
-                              <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="range" form="unqualified"/>
-                              <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="movingTimeInterval" form="unqualified"/>
                             </xsd:sequence>
                           </xsd:complexType>
                         </xsd:element>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="shootingTimeInterval" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="sShootingDirection" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="isMoving" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="sMovingDirection" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="range" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="movingTimeInterval" form="unqualified"/>
                       </xsd:sequence>
                     </xsd:complexType>
                   </xsd:element>
@@ -693,27 +696,27 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="9" Name="SavableLevel_映射" RootElement="SavableLevel" SchemaID="Schema4" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="7" DataBindingLoadMode="1"/>
+  <Map ID="10" Name="SavableLevel_映射" RootElement="SavableLevel" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="8" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表4" displayName="表4" ref="A1:C401" tableType="xml" totalsRowShown="0" connectionId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表4" displayName="表4" ref="A1:C401" tableType="xml" totalsRowShown="0" connectionId="8">
   <autoFilter ref="A1:C401"/>
   <tableColumns count="3">
     <tableColumn id="1" uniqueName="x" name="x">
       <calculatedColumnFormula>INT((ROW()-2)/20)</calculatedColumnFormula>
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/tMap/Tile/vTilePosition/x" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/tMap/Tile/vTilePosition/x" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="y" name="y">
       <calculatedColumnFormula>MOD(ROW()-2,20)</calculatedColumnFormula>
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/tMap/Tile/vTilePosition/y" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/tMap/Tile/vTilePosition/y" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="iTileType" name="iTileType" dataDxfId="0">
       <calculatedColumnFormula>INDEX('map source data'!$A$1:$T$20,$F$8-('exportable data'!B2),'exportable data'!A2+1)</calculatedColumnFormula>
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/tMap/Tile/iTileType" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/tMap/Tile/iTileType" xmlDataType="integer"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -721,29 +724,29 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="表20" displayName="表20" ref="M1:S5" tableType="xml" totalsRowShown="0" connectionId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="表20" displayName="表20" ref="M1:S5" tableType="xml" totalsRowShown="0" connectionId="8">
   <autoFilter ref="M1:S5"/>
   <tableColumns count="7">
     <tableColumn id="1" uniqueName="x" name="vPositionX">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/pPushers/PusherInXML/vPosition/x" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/pPushers/PusherInXML/vPosition/x" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="y" name="vPositionY">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/pPushers/PusherInXML/vPosition/y" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/pPushers/PusherInXML/vPosition/y" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="isControlled" name="isControlled">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/pPushers/PusherInXML/isControlled" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/pPushers/PusherInXML/isControlled" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="sDirection" name="sDirection">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/pPushers/PusherInXML/sDirection" xmlDataType="string"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/pPushers/PusherInXML/sDirection" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="5" uniqueName="range" name="range">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/pPushers/PusherInXML/range" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/pPushers/PusherInXML/range" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="6" uniqueName="ID" name="ID">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/pPushers/PusherInXML/ID" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/pPushers/PusherInXML/ID" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="7" uniqueName="timeInterval" name="timeInterval">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/pPushers/PusherInXML/timeInterval" xmlDataType="double"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/pPushers/PusherInXML/timeInterval" xmlDataType="double"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -751,20 +754,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="AA1:AD3" tableType="xml" totalsRowShown="0" connectionId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="AA1:AD3" tableType="xml" totalsRowShown="0" connectionId="8">
   <autoFilter ref="AA1:AD3"/>
   <tableColumns count="4">
     <tableColumn id="1" uniqueName="x" name="vPositionX">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/dDoors/DoorInXML/vPosition/x" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/dDoors/DoorInXML/vPosition/x" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="y" name="vPositionY">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/dDoors/DoorInXML/vPosition/y" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/dDoors/DoorInXML/vPosition/y" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="iID" name="ID">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/dDoors/DoorInXML/iID" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/dDoors/DoorInXML/iID" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="triggerNumber" name="triggerNumber">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/dDoors/DoorInXML/triggerNumber" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/dDoors/DoorInXML/triggerNumber" xmlDataType="integer"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -772,14 +775,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="表12" displayName="表12" ref="I1:J3" tableType="xml" totalsRowShown="0" connectionId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="表12" displayName="表12" ref="I1:J3" tableType="xml" totalsRowShown="0" connectionId="8">
   <autoFilter ref="I1:J3"/>
   <tableColumns count="2">
     <tableColumn id="1" uniqueName="x" name="vPositionX">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/sStars/StarInXML/vPosition/x" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/sStars/StarInXML/vPosition/x" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="y" name="vPositionY">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/sStars/StarInXML/vPosition/y" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/sStars/StarInXML/vPosition/y" xmlDataType="integer"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -787,17 +790,17 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="表13" displayName="表13" ref="AG1:AI3" tableType="xml" totalsRowShown="0" connectionId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="表13" displayName="表13" ref="AG1:AI3" tableType="xml" totalsRowShown="0" connectionId="8">
   <autoFilter ref="AG1:AI3"/>
   <tableColumns count="3">
     <tableColumn id="1" uniqueName="x" name="vPositionX">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/StepTriggers/StepTriggerInXML/vPosition/x" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/StepTriggers/StepTriggerInXML/vPosition/x" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="y" name="vPositionY">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/StepTriggers/StepTriggerInXML/vPosition/y" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/StepTriggers/StepTriggerInXML/vPosition/y" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="iID" name="ID">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/StepTriggers/StepTriggerInXML/iID" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/StepTriggers/StepTriggerInXML/iID" xmlDataType="integer"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -805,17 +808,17 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="表14" displayName="表14" ref="V1:X3" tableType="xml" totalsRowShown="0" connectionId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="表14" displayName="表14" ref="V1:X3" tableType="xml" totalsRowShown="0" connectionId="8">
   <autoFilter ref="V1:X3"/>
   <tableColumns count="3">
     <tableColumn id="1" uniqueName="x" name="vPositionX">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/StayTriggers/StayTriggerInXML/vPosition/x" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/StayTriggers/StayTriggerInXML/vPosition/x" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="y" name="vPositionY">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/StayTriggers/StayTriggerInXML/vPosition/y" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/StayTriggers/StayTriggerInXML/vPosition/y" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="iID" name="ID">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/StayTriggers/StayTriggerInXML/iID" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/StayTriggers/StayTriggerInXML/iID" xmlDataType="integer"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -823,32 +826,32 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="表15" displayName="表15" ref="AL1:AS3" tableType="xml" totalsRowShown="0" connectionId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="表15" displayName="表15" ref="AL1:AS3" tableType="xml" totalsRowShown="0" connectionId="8">
   <autoFilter ref="AL1:AS3"/>
   <tableColumns count="8">
     <tableColumn id="1" uniqueName="x" name="vPositionX">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/Shooters/ShooterInXML/vPosition/x" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/sShooters/ShooterInXML/vPosition/x" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="y" name="vPositionY">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/Shooters/ShooterInXML/vPosition/y" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/sShooters/ShooterInXML/vPosition/y" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="shootingTimeInterval" name="shootingTimeInterval">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/Shooters/ShooterInXML/vPosition/shootingTimeInterval" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/sShooters/ShooterInXML/shootingTimeInterval" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="sShootingDirection" name="sShootingDirection">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/Shooters/ShooterInXML/vPosition/sShootingDirection" xmlDataType="string"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/sShooters/ShooterInXML/sShootingDirection" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="5" uniqueName="isMoving" name="isMoving">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/Shooters/ShooterInXML/vPosition/isMoving" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/sShooters/ShooterInXML/isMoving" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="6" uniqueName="sMovingDirection" name="sMovingDirection">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/Shooters/ShooterInXML/vPosition/sMovingDirection" xmlDataType="string"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/sShooters/ShooterInXML/sMovingDirection" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="7" uniqueName="range" name="range">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/Shooters/ShooterInXML/vPosition/range" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/sShooters/ShooterInXML/range" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="8" uniqueName="movingTimeInterval" name="movingTimeInterval">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/Shooters/ShooterInXML/vPosition/movingTimeInterval" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/sShooters/ShooterInXML/movingTimeInterval" xmlDataType="integer"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -856,20 +859,20 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="表16" displayName="表16" ref="AV1:AY4" tableType="xml" totalsRowShown="0" connectionId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="表16" displayName="表16" ref="AV1:AY4" tableType="xml" totalsRowShown="0" connectionId="8">
   <autoFilter ref="AV1:AY4"/>
   <tableColumns count="4">
     <tableColumn id="1" uniqueName="x" name="vCheckPoint1PositionX">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/cCheckPoints/CheckPointInXML/vCheckPoint1Position/x" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/cCheckPoints/CheckPointInXML/vCheckPoint1Position/x" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="y" name="vCheckPoint1PositionY">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/cCheckPoints/CheckPointInXML/vCheckPoint1Position/y" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/cCheckPoints/CheckPointInXML/vCheckPoint1Position/y" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="x" name="vCheckPoint2PositionX">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/cCheckPoints/CheckPointInXML/vCheckPoint2Position/x" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/cCheckPoints/CheckPointInXML/vCheckPoint2Position/x" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="y" name="vCheckPoint2PositionY">
-      <xmlColumnPr mapId="9" xpath="/SavableLevel/cCheckPoints/CheckPointInXML/vCheckPoint2Position/y" xmlDataType="integer"/>
+      <xmlColumnPr mapId="10" xpath="/SavableLevel/cCheckPoints/CheckPointInXML/vCheckPoint2Position/y" xmlDataType="integer"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -878,44 +881,44 @@
 
 <file path=xl/tables/tableSingleCells1.xml><?xml version="1.0" encoding="utf-8"?>
 <singleXmlCells xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <singleXmlCell id="3" r="F1" connectionId="7">
+  <singleXmlCell id="2" r="F1" connectionId="8">
     <xmlCellPr id="1" uniqueName="sLevelName">
-      <xmlPr mapId="9" xpath="/SavableLevel/sLevelName" xmlDataType="string"/>
+      <xmlPr mapId="10" xpath="/SavableLevel/sLevelName" xmlDataType="string"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="5" r="F2" connectionId="7">
+  <singleXmlCell id="3" r="F2" connectionId="8">
     <xmlCellPr id="1" uniqueName="iLevelType">
-      <xmlPr mapId="9" xpath="/SavableLevel/iLevelType" xmlDataType="integer"/>
+      <xmlPr mapId="10" xpath="/SavableLevel/iLevelType" xmlDataType="integer"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="6" r="F3" connectionId="7">
+  <singleXmlCell id="5" r="F3" connectionId="8">
     <xmlCellPr id="1" uniqueName="x">
-      <xmlPr mapId="9" xpath="/SavableLevel/vChar1StartPos/x" xmlDataType="integer"/>
+      <xmlPr mapId="10" xpath="/SavableLevel/vChar1StartPos/x" xmlDataType="integer"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="7" r="F4" connectionId="7">
+  <singleXmlCell id="6" r="F4" connectionId="8">
     <xmlCellPr id="1" uniqueName="y">
-      <xmlPr mapId="9" xpath="/SavableLevel/vChar1StartPos/y" xmlDataType="integer"/>
+      <xmlPr mapId="10" xpath="/SavableLevel/vChar1StartPos/y" xmlDataType="integer"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="8" r="F5" connectionId="7">
+  <singleXmlCell id="7" r="F5" connectionId="8">
     <xmlCellPr id="1" uniqueName="x">
-      <xmlPr mapId="9" xpath="/SavableLevel/vChar2StartPos/x" xmlDataType="integer"/>
+      <xmlPr mapId="10" xpath="/SavableLevel/vChar2StartPos/x" xmlDataType="integer"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="9" r="F6" connectionId="7">
+  <singleXmlCell id="8" r="F6" connectionId="8">
     <xmlCellPr id="1" uniqueName="y">
-      <xmlPr mapId="9" xpath="/SavableLevel/vChar2StartPos/y" xmlDataType="integer"/>
+      <xmlPr mapId="10" xpath="/SavableLevel/vChar2StartPos/y" xmlDataType="integer"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="10" r="F7" connectionId="7">
+  <singleXmlCell id="9" r="F7" connectionId="8">
     <xmlCellPr id="1" uniqueName="x">
-      <xmlPr mapId="9" xpath="/SavableLevel/vDim/x" xmlDataType="integer"/>
+      <xmlPr mapId="10" xpath="/SavableLevel/vDim/x" xmlDataType="integer"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="11" r="F8" connectionId="7">
+  <singleXmlCell id="10" r="F8" connectionId="8">
     <xmlCellPr id="1" uniqueName="y">
-      <xmlPr mapId="9" xpath="/SavableLevel/vDim/y" xmlDataType="integer"/>
+      <xmlPr mapId="10" xpath="/SavableLevel/vDim/y" xmlDataType="integer"/>
     </xmlCellPr>
   </singleXmlCell>
 </singleXmlCells>
@@ -2468,7 +2471,7 @@
   <dimension ref="A1:AY401"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.75" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2722,10 +2725,10 @@
         <v>1</v>
       </c>
       <c r="AL2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AM2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AN2">
         <v>4</v>
@@ -2734,7 +2737,7 @@
         <v>48</v>
       </c>
       <c r="AP2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ2" s="1" t="s">
         <v>49</v>
@@ -2837,8 +2840,30 @@
       <c r="AI3">
         <v>2</v>
       </c>
-      <c r="AO3" s="1"/>
-      <c r="AQ3" s="1"/>
+      <c r="AL3">
+        <v>12</v>
+      </c>
+      <c r="AM3">
+        <v>10</v>
+      </c>
+      <c r="AN3">
+        <v>4</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP3">
+        <v>1</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR3">
+        <v>2</v>
+      </c>
+      <c r="AS3">
+        <v>1</v>
+      </c>
       <c r="AU3" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
check point (manager version. will be merged into worldmanager)
</commit_message>
<xml_diff>
--- a/BlockTileSystem/Assets/Levels/map_schema.xlsx
+++ b/BlockTileSystem/Assets/Levels/map_schema.xlsx
@@ -1220,7 +1220,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2048,10 +2048,10 @@
         <v>2</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -2476,8 +2476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY401"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.75" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2674,10 +2674,10 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J2">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M2" s="1">
         <v>5</v>
@@ -2758,13 +2758,13 @@
         <v>42</v>
       </c>
       <c r="AV2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AW2">
         <v>5</v>
       </c>
       <c r="AX2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AY2">
         <v>6</v>
@@ -2790,10 +2790,10 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M3" s="1">
         <v>6</v>
@@ -2874,13 +2874,13 @@
         <v>43</v>
       </c>
       <c r="AV3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AW3">
         <v>7</v>
       </c>
       <c r="AX3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AY3">
         <v>8</v>
@@ -3028,7 +3028,7 @@
         <v>10</v>
       </c>
       <c r="F8">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:51" x14ac:dyDescent="0.15">
@@ -3152,7 +3152,7 @@
       </c>
       <c r="B17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C17">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B17),A17+1)</f>
@@ -3166,7 +3166,7 @@
       </c>
       <c r="B18">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C18">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B18),A18+1)</f>
@@ -3180,7 +3180,7 @@
       </c>
       <c r="B19">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C19">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B19),A19+1)</f>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="B20">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C20">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B20),A20+1)</f>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="B21">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C21">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B21),A21+1)</f>
@@ -3222,11 +3222,11 @@
       </c>
       <c r="B22">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C22">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B22),A22+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
@@ -3236,7 +3236,7 @@
       </c>
       <c r="B23">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C23">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B23),A23+1)</f>
@@ -3250,7 +3250,7 @@
       </c>
       <c r="B24">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C24">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B24),A24+1)</f>
@@ -3264,7 +3264,7 @@
       </c>
       <c r="B25">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C25">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B25),A25+1)</f>
@@ -3278,7 +3278,7 @@
       </c>
       <c r="B26">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C26">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B26),A26+1)</f>
@@ -3292,7 +3292,7 @@
       </c>
       <c r="B27">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C27">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B27),A27+1)</f>
@@ -3306,7 +3306,7 @@
       </c>
       <c r="B28">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C28">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B28),A28+1)</f>
@@ -3320,7 +3320,7 @@
       </c>
       <c r="B29">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C29">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B29),A29+1)</f>
@@ -3334,7 +3334,7 @@
       </c>
       <c r="B30">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C30">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B30),A30+1)</f>
@@ -3348,11 +3348,11 @@
       </c>
       <c r="B31">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C31">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B31),A31+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
@@ -3362,7 +3362,7 @@
       </c>
       <c r="B32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C32">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B32),A32+1)</f>
@@ -3376,7 +3376,7 @@
       </c>
       <c r="B33">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C33">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B33),A33+1)</f>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="B34">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C34">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B34),A34+1)</f>
@@ -3404,7 +3404,7 @@
       </c>
       <c r="B35">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C35">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B35),A35+1)</f>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="B36">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C36">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B36),A36+1)</f>
@@ -3432,7 +3432,7 @@
       </c>
       <c r="B37">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C37">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B37),A37+1)</f>
@@ -3446,7 +3446,7 @@
       </c>
       <c r="B38">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C38">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B38),A38+1)</f>
@@ -3460,7 +3460,7 @@
       </c>
       <c r="B39">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C39">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B39),A39+1)</f>
@@ -3474,7 +3474,7 @@
       </c>
       <c r="B40">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C40">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B40),A40+1)</f>
@@ -3488,11 +3488,11 @@
       </c>
       <c r="B41">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C41">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B41),A41+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
@@ -3502,11 +3502,11 @@
       </c>
       <c r="B42">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C42">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B42),A42+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
@@ -3516,7 +3516,7 @@
       </c>
       <c r="B43">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C43">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B43),A43+1)</f>
@@ -3530,7 +3530,7 @@
       </c>
       <c r="B44">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C44">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B44),A44+1)</f>
@@ -3544,7 +3544,7 @@
       </c>
       <c r="B45">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C45">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B45),A45+1)</f>
@@ -3558,11 +3558,11 @@
       </c>
       <c r="B46">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C46">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B46),A46+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
@@ -3572,7 +3572,7 @@
       </c>
       <c r="B47">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C47">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B47),A47+1)</f>
@@ -3586,7 +3586,7 @@
       </c>
       <c r="B48">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C48">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B48),A48+1)</f>
@@ -3600,7 +3600,7 @@
       </c>
       <c r="B49">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C49">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B49),A49+1)</f>
@@ -3614,7 +3614,7 @@
       </c>
       <c r="B50">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C50">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B50),A50+1)</f>
@@ -3628,7 +3628,7 @@
       </c>
       <c r="B51">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C51">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B51),A51+1)</f>
@@ -3642,7 +3642,7 @@
       </c>
       <c r="B52">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C52">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B52),A52+1)</f>
@@ -3656,7 +3656,7 @@
       </c>
       <c r="B53">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C53">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B53),A53+1)</f>
@@ -3670,7 +3670,7 @@
       </c>
       <c r="B54">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C54">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B54),A54+1)</f>
@@ -3684,7 +3684,7 @@
       </c>
       <c r="B55">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C55">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B55),A55+1)</f>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="B56">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C56">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B56),A56+1)</f>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="B57">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C57">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B57),A57+1)</f>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="B58">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C58">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B58),A58+1)</f>
@@ -3740,7 +3740,7 @@
       </c>
       <c r="B59">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C59">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B59),A59+1)</f>
@@ -3754,7 +3754,7 @@
       </c>
       <c r="B60">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C60">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B60),A60+1)</f>
@@ -3768,7 +3768,7 @@
       </c>
       <c r="B61">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C61">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B61),A61+1)</f>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="C62">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B62),A62+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
@@ -3982,7 +3982,7 @@
       </c>
       <c r="C76">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B76),A76+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
@@ -3992,7 +3992,7 @@
       </c>
       <c r="B77">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C77">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B77),A77+1)</f>
@@ -4006,7 +4006,7 @@
       </c>
       <c r="B78">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C78">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B78),A78+1)</f>
@@ -4020,7 +4020,7 @@
       </c>
       <c r="B79">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C79">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B79),A79+1)</f>
@@ -4034,7 +4034,7 @@
       </c>
       <c r="B80">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C80">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B80),A80+1)</f>
@@ -4048,11 +4048,11 @@
       </c>
       <c r="B81">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C81">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B81),A81+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
@@ -4062,11 +4062,11 @@
       </c>
       <c r="B82">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C82">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B82),A82+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
@@ -4076,11 +4076,11 @@
       </c>
       <c r="B83">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C83">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B83),A83+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
@@ -4090,11 +4090,11 @@
       </c>
       <c r="B84">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C84">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B84),A84+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
@@ -4104,11 +4104,11 @@
       </c>
       <c r="B85">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C85">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B85),A85+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
@@ -4118,11 +4118,11 @@
       </c>
       <c r="B86">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C86">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B86),A86+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
@@ -4132,11 +4132,11 @@
       </c>
       <c r="B87">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C87">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B87),A87+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
@@ -4146,11 +4146,11 @@
       </c>
       <c r="B88">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C88">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B88),A88+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
@@ -4160,7 +4160,7 @@
       </c>
       <c r="B89">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C89">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B89),A89+1)</f>
@@ -4174,7 +4174,7 @@
       </c>
       <c r="B90">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C90">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B90),A90+1)</f>
@@ -4188,11 +4188,11 @@
       </c>
       <c r="B91">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C91">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B91),A91+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
@@ -4202,11 +4202,11 @@
       </c>
       <c r="B92">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C92">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B92),A92+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.15">
@@ -4216,11 +4216,11 @@
       </c>
       <c r="B93">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C93">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B93),A93+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.15">
@@ -4230,7 +4230,7 @@
       </c>
       <c r="B94">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C94">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B94),A94+1)</f>
@@ -4244,7 +4244,7 @@
       </c>
       <c r="B95">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C95">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B95),A95+1)</f>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="B96">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C96">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B96),A96+1)</f>
@@ -4272,7 +4272,7 @@
       </c>
       <c r="B97">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C97">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B97),A97+1)</f>
@@ -4286,7 +4286,7 @@
       </c>
       <c r="B98">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C98">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B98),A98+1)</f>
@@ -4300,7 +4300,7 @@
       </c>
       <c r="B99">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C99">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B99),A99+1)</f>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="B100">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C100">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B100),A100+1)</f>
@@ -4328,11 +4328,11 @@
       </c>
       <c r="B101">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C101">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B101),A101+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.15">
@@ -4342,11 +4342,11 @@
       </c>
       <c r="B102">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C102">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B102),A102+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.15">
@@ -4356,7 +4356,7 @@
       </c>
       <c r="B103">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C103">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B103),A103+1)</f>
@@ -4370,7 +4370,7 @@
       </c>
       <c r="B104">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C104">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B104),A104+1)</f>
@@ -4384,7 +4384,7 @@
       </c>
       <c r="B105">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C105">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B105),A105+1)</f>
@@ -4398,11 +4398,11 @@
       </c>
       <c r="B106">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C106">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B106),A106+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.15">
@@ -4412,7 +4412,7 @@
       </c>
       <c r="B107">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C107">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B107),A107+1)</f>
@@ -4426,11 +4426,11 @@
       </c>
       <c r="B108">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C108">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B108),A108+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.15">
@@ -4440,7 +4440,7 @@
       </c>
       <c r="B109">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C109">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B109),A109+1)</f>
@@ -4454,7 +4454,7 @@
       </c>
       <c r="B110">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C110">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B110),A110+1)</f>
@@ -4468,7 +4468,7 @@
       </c>
       <c r="B111">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C111">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B111),A111+1)</f>
@@ -4482,7 +4482,7 @@
       </c>
       <c r="B112">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C112">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B112),A112+1)</f>
@@ -4496,7 +4496,7 @@
       </c>
       <c r="B113">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C113">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B113),A113+1)</f>
@@ -4510,7 +4510,7 @@
       </c>
       <c r="B114">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C114">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B114),A114+1)</f>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="B115">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C115">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B115),A115+1)</f>
@@ -4538,7 +4538,7 @@
       </c>
       <c r="B116">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C116">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B116),A116+1)</f>
@@ -4552,7 +4552,7 @@
       </c>
       <c r="B117">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C117">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B117),A117+1)</f>
@@ -4566,7 +4566,7 @@
       </c>
       <c r="B118">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C118">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B118),A118+1)</f>
@@ -4580,7 +4580,7 @@
       </c>
       <c r="B119">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C119">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B119),A119+1)</f>
@@ -4594,7 +4594,7 @@
       </c>
       <c r="B120">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C120">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B120),A120+1)</f>
@@ -4608,7 +4608,7 @@
       </c>
       <c r="B121">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C121">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B121),A121+1)</f>
@@ -4626,7 +4626,7 @@
       </c>
       <c r="C122">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B122),A122+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.15">
@@ -4640,7 +4640,7 @@
       </c>
       <c r="C123">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B123),A123+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.15">
@@ -4822,7 +4822,7 @@
       </c>
       <c r="C136">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B136),A136+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.15">
@@ -4832,7 +4832,7 @@
       </c>
       <c r="B137">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C137">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B137),A137+1)</f>
@@ -4846,11 +4846,11 @@
       </c>
       <c r="B138">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C138">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B138),A138+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
@@ -4860,7 +4860,7 @@
       </c>
       <c r="B139">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C139">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B139),A139+1)</f>
@@ -4874,7 +4874,7 @@
       </c>
       <c r="B140">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C140">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B140),A140+1)</f>
@@ -4888,11 +4888,11 @@
       </c>
       <c r="B141">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C141">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B141),A141+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
@@ -4902,11 +4902,11 @@
       </c>
       <c r="B142">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C142">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B142),A142+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.15">
@@ -4916,7 +4916,7 @@
       </c>
       <c r="B143">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C143">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B143),A143+1)</f>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="B144">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C144">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B144),A144+1)</f>
@@ -4944,7 +4944,7 @@
       </c>
       <c r="B145">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C145">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B145),A145+1)</f>
@@ -4958,7 +4958,7 @@
       </c>
       <c r="B146">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C146">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B146),A146+1)</f>
@@ -4972,7 +4972,7 @@
       </c>
       <c r="B147">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C147">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B147),A147+1)</f>
@@ -4986,7 +4986,7 @@
       </c>
       <c r="B148">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C148">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B148),A148+1)</f>
@@ -5000,7 +5000,7 @@
       </c>
       <c r="B149">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C149">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B149),A149+1)</f>
@@ -5014,7 +5014,7 @@
       </c>
       <c r="B150">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C150">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B150),A150+1)</f>
@@ -5028,11 +5028,11 @@
       </c>
       <c r="B151">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C151">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B151),A151+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.15">
@@ -5042,7 +5042,7 @@
       </c>
       <c r="B152">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C152">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B152),A152+1)</f>
@@ -5056,7 +5056,7 @@
       </c>
       <c r="B153">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C153">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B153),A153+1)</f>
@@ -5070,7 +5070,7 @@
       </c>
       <c r="B154">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C154">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B154),A154+1)</f>
@@ -5084,7 +5084,7 @@
       </c>
       <c r="B155">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C155">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B155),A155+1)</f>
@@ -5098,7 +5098,7 @@
       </c>
       <c r="B156">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C156">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B156),A156+1)</f>
@@ -5112,7 +5112,7 @@
       </c>
       <c r="B157">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C157">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B157),A157+1)</f>
@@ -5126,7 +5126,7 @@
       </c>
       <c r="B158">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C158">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B158),A158+1)</f>
@@ -5140,7 +5140,7 @@
       </c>
       <c r="B159">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C159">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B159),A159+1)</f>
@@ -5154,7 +5154,7 @@
       </c>
       <c r="B160">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C160">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B160),A160+1)</f>
@@ -5168,11 +5168,11 @@
       </c>
       <c r="B161">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C161">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B161),A161+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.15">
@@ -5182,11 +5182,11 @@
       </c>
       <c r="B162">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C162">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B162),A162+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.15">
@@ -5196,7 +5196,7 @@
       </c>
       <c r="B163">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C163">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B163),A163+1)</f>
@@ -5210,7 +5210,7 @@
       </c>
       <c r="B164">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C164">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B164),A164+1)</f>
@@ -5224,7 +5224,7 @@
       </c>
       <c r="B165">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C165">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B165),A165+1)</f>
@@ -5238,11 +5238,11 @@
       </c>
       <c r="B166">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C166">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B166),A166+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.15">
@@ -5252,7 +5252,7 @@
       </c>
       <c r="B167">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C167">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B167),A167+1)</f>
@@ -5266,7 +5266,7 @@
       </c>
       <c r="B168">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C168">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B168),A168+1)</f>
@@ -5280,7 +5280,7 @@
       </c>
       <c r="B169">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C169">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B169),A169+1)</f>
@@ -5294,7 +5294,7 @@
       </c>
       <c r="B170">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C170">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B170),A170+1)</f>
@@ -5308,7 +5308,7 @@
       </c>
       <c r="B171">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C171">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B171),A171+1)</f>
@@ -5322,7 +5322,7 @@
       </c>
       <c r="B172">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C172">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B172),A172+1)</f>
@@ -5336,7 +5336,7 @@
       </c>
       <c r="B173">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C173">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B173),A173+1)</f>
@@ -5350,7 +5350,7 @@
       </c>
       <c r="B174">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C174">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B174),A174+1)</f>
@@ -5364,7 +5364,7 @@
       </c>
       <c r="B175">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C175">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B175),A175+1)</f>
@@ -5378,7 +5378,7 @@
       </c>
       <c r="B176">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C176">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B176),A176+1)</f>
@@ -5392,7 +5392,7 @@
       </c>
       <c r="B177">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C177">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B177),A177+1)</f>
@@ -5406,7 +5406,7 @@
       </c>
       <c r="B178">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C178">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B178),A178+1)</f>
@@ -5420,7 +5420,7 @@
       </c>
       <c r="B179">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C179">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B179),A179+1)</f>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="B180">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C180">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B180),A180+1)</f>
@@ -5448,7 +5448,7 @@
       </c>
       <c r="B181">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C181">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B181),A181+1)</f>
@@ -5466,7 +5466,7 @@
       </c>
       <c r="C182">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B182),A182+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.15">
@@ -5662,7 +5662,7 @@
       </c>
       <c r="C196">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B196),A196+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.15">
@@ -5672,7 +5672,7 @@
       </c>
       <c r="B197">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C197">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B197),A197+1)</f>
@@ -5686,7 +5686,7 @@
       </c>
       <c r="B198">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C198">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B198),A198+1)</f>
@@ -5700,7 +5700,7 @@
       </c>
       <c r="B199">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C199">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B199),A199+1)</f>
@@ -5714,7 +5714,7 @@
       </c>
       <c r="B200">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C200">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B200),A200+1)</f>
@@ -5728,11 +5728,11 @@
       </c>
       <c r="B201">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C201">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B201),A201+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.15">
@@ -5742,11 +5742,11 @@
       </c>
       <c r="B202">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C202">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B202),A202+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.15">
@@ -5756,7 +5756,7 @@
       </c>
       <c r="B203">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C203">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B203),A203+1)</f>
@@ -5770,7 +5770,7 @@
       </c>
       <c r="B204">
         <f t="shared" si="7"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C204">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B204),A204+1)</f>
@@ -5784,7 +5784,7 @@
       </c>
       <c r="B205">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C205">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B205),A205+1)</f>
@@ -5798,7 +5798,7 @@
       </c>
       <c r="B206">
         <f t="shared" si="7"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C206">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B206),A206+1)</f>
@@ -5812,7 +5812,7 @@
       </c>
       <c r="B207">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C207">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B207),A207+1)</f>
@@ -5826,7 +5826,7 @@
       </c>
       <c r="B208">
         <f t="shared" si="7"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C208">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B208),A208+1)</f>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="B209">
         <f t="shared" si="7"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C209">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B209),A209+1)</f>
@@ -5854,7 +5854,7 @@
       </c>
       <c r="B210">
         <f t="shared" si="7"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C210">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B210),A210+1)</f>
@@ -5868,11 +5868,11 @@
       </c>
       <c r="B211">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C211">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B211),A211+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.15">
@@ -5882,7 +5882,7 @@
       </c>
       <c r="B212">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C212">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B212),A212+1)</f>
@@ -5896,7 +5896,7 @@
       </c>
       <c r="B213">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C213">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B213),A213+1)</f>
@@ -5910,7 +5910,7 @@
       </c>
       <c r="B214">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C214">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B214),A214+1)</f>
@@ -5924,7 +5924,7 @@
       </c>
       <c r="B215">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C215">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B215),A215+1)</f>
@@ -5938,7 +5938,7 @@
       </c>
       <c r="B216">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C216">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B216),A216+1)</f>
@@ -5952,7 +5952,7 @@
       </c>
       <c r="B217">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C217">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B217),A217+1)</f>
@@ -5966,7 +5966,7 @@
       </c>
       <c r="B218">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C218">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B218),A218+1)</f>
@@ -5980,7 +5980,7 @@
       </c>
       <c r="B219">
         <f t="shared" si="7"/>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C219">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B219),A219+1)</f>
@@ -5994,7 +5994,7 @@
       </c>
       <c r="B220">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C220">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B220),A220+1)</f>
@@ -6008,11 +6008,11 @@
       </c>
       <c r="B221">
         <f t="shared" si="7"/>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C221">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B221),A221+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.15">
@@ -6022,11 +6022,11 @@
       </c>
       <c r="B222">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C222">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B222),A222+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.15">
@@ -6036,7 +6036,7 @@
       </c>
       <c r="B223">
         <f t="shared" si="7"/>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C223">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B223),A223+1)</f>
@@ -6050,7 +6050,7 @@
       </c>
       <c r="B224">
         <f t="shared" si="7"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C224">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B224),A224+1)</f>
@@ -6064,7 +6064,7 @@
       </c>
       <c r="B225">
         <f t="shared" si="7"/>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C225">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B225),A225+1)</f>
@@ -6078,11 +6078,11 @@
       </c>
       <c r="B226">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C226">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B226),A226+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.15">
@@ -6092,7 +6092,7 @@
       </c>
       <c r="B227">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C227">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B227),A227+1)</f>
@@ -6106,7 +6106,7 @@
       </c>
       <c r="B228">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C228">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B228),A228+1)</f>
@@ -6120,7 +6120,7 @@
       </c>
       <c r="B229">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C229">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B229),A229+1)</f>
@@ -6134,7 +6134,7 @@
       </c>
       <c r="B230">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C230">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B230),A230+1)</f>
@@ -6148,7 +6148,7 @@
       </c>
       <c r="B231">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C231">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B231),A231+1)</f>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="B232">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C232">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B232),A232+1)</f>
@@ -6176,7 +6176,7 @@
       </c>
       <c r="B233">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C233">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B233),A233+1)</f>
@@ -6190,7 +6190,7 @@
       </c>
       <c r="B234">
         <f t="shared" si="7"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C234">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B234),A234+1)</f>
@@ -6204,7 +6204,7 @@
       </c>
       <c r="B235">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C235">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B235),A235+1)</f>
@@ -6218,7 +6218,7 @@
       </c>
       <c r="B236">
         <f t="shared" si="7"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C236">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B236),A236+1)</f>
@@ -6232,7 +6232,7 @@
       </c>
       <c r="B237">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C237">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B237),A237+1)</f>
@@ -6246,7 +6246,7 @@
       </c>
       <c r="B238">
         <f t="shared" si="7"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C238">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B238),A238+1)</f>
@@ -6260,7 +6260,7 @@
       </c>
       <c r="B239">
         <f t="shared" si="7"/>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C239">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B239),A239+1)</f>
@@ -6274,7 +6274,7 @@
       </c>
       <c r="B240">
         <f t="shared" si="7"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C240">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B240),A240+1)</f>
@@ -6288,7 +6288,7 @@
       </c>
       <c r="B241">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C241">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B241),A241+1)</f>
@@ -6306,7 +6306,7 @@
       </c>
       <c r="C242">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B242),A242+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.15">
@@ -6502,7 +6502,7 @@
       </c>
       <c r="C256">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B256),A256+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.15">
@@ -6512,7 +6512,7 @@
       </c>
       <c r="B257">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C257">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B257),A257+1)</f>
@@ -6526,7 +6526,7 @@
       </c>
       <c r="B258">
         <f t="shared" ref="B258:B321" si="9">MOD(ROW()-2,$F$8)</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C258">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B258),A258+1)</f>
@@ -6540,7 +6540,7 @@
       </c>
       <c r="B259">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C259">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B259),A259+1)</f>
@@ -6554,7 +6554,7 @@
       </c>
       <c r="B260">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C260">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B260),A260+1)</f>
@@ -6568,11 +6568,11 @@
       </c>
       <c r="B261">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C261">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B261),A261+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.15">
@@ -6582,11 +6582,11 @@
       </c>
       <c r="B262">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C262">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B262),A262+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.15">
@@ -6596,7 +6596,7 @@
       </c>
       <c r="B263">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C263">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B263),A263+1)</f>
@@ -6610,7 +6610,7 @@
       </c>
       <c r="B264">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C264">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B264),A264+1)</f>
@@ -6624,7 +6624,7 @@
       </c>
       <c r="B265">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C265">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B265),A265+1)</f>
@@ -6638,7 +6638,7 @@
       </c>
       <c r="B266">
         <f t="shared" si="9"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C266">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B266),A266+1)</f>
@@ -6652,7 +6652,7 @@
       </c>
       <c r="B267">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C267">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B267),A267+1)</f>
@@ -6666,7 +6666,7 @@
       </c>
       <c r="B268">
         <f t="shared" si="9"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C268">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B268),A268+1)</f>
@@ -6680,7 +6680,7 @@
       </c>
       <c r="B269">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C269">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B269),A269+1)</f>
@@ -6694,7 +6694,7 @@
       </c>
       <c r="B270">
         <f t="shared" si="9"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C270">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B270),A270+1)</f>
@@ -6708,11 +6708,11 @@
       </c>
       <c r="B271">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C271">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B271),A271+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.15">
@@ -6722,7 +6722,7 @@
       </c>
       <c r="B272">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C272">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B272),A272+1)</f>
@@ -6736,7 +6736,7 @@
       </c>
       <c r="B273">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C273">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B273),A273+1)</f>
@@ -6750,7 +6750,7 @@
       </c>
       <c r="B274">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C274">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B274),A274+1)</f>
@@ -6764,7 +6764,7 @@
       </c>
       <c r="B275">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C275">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B275),A275+1)</f>
@@ -6778,7 +6778,7 @@
       </c>
       <c r="B276">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C276">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B276),A276+1)</f>
@@ -6792,7 +6792,7 @@
       </c>
       <c r="B277">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C277">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B277),A277+1)</f>
@@ -6806,7 +6806,7 @@
       </c>
       <c r="B278">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C278">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B278),A278+1)</f>
@@ -6820,7 +6820,7 @@
       </c>
       <c r="B279">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C279">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B279),A279+1)</f>
@@ -6834,7 +6834,7 @@
       </c>
       <c r="B280">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C280">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B280),A280+1)</f>
@@ -6848,11 +6848,11 @@
       </c>
       <c r="B281">
         <f t="shared" si="9"/>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C281">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B281),A281+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.15">
@@ -6862,11 +6862,11 @@
       </c>
       <c r="B282">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C282">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B282),A282+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.15">
@@ -6876,7 +6876,7 @@
       </c>
       <c r="B283">
         <f t="shared" si="9"/>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C283">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B283),A283+1)</f>
@@ -6890,7 +6890,7 @@
       </c>
       <c r="B284">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C284">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B284),A284+1)</f>
@@ -6904,7 +6904,7 @@
       </c>
       <c r="B285">
         <f t="shared" si="9"/>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C285">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B285),A285+1)</f>
@@ -6918,11 +6918,11 @@
       </c>
       <c r="B286">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C286">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B286),A286+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.15">
@@ -6932,7 +6932,7 @@
       </c>
       <c r="B287">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C287">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B287),A287+1)</f>
@@ -6946,7 +6946,7 @@
       </c>
       <c r="B288">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C288">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B288),A288+1)</f>
@@ -6960,7 +6960,7 @@
       </c>
       <c r="B289">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C289">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B289),A289+1)</f>
@@ -6974,7 +6974,7 @@
       </c>
       <c r="B290">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C290">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B290),A290+1)</f>
@@ -6988,7 +6988,7 @@
       </c>
       <c r="B291">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C291">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B291),A291+1)</f>
@@ -7002,7 +7002,7 @@
       </c>
       <c r="B292">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C292">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B292),A292+1)</f>
@@ -7016,7 +7016,7 @@
       </c>
       <c r="B293">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C293">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B293),A293+1)</f>
@@ -7030,7 +7030,7 @@
       </c>
       <c r="B294">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C294">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B294),A294+1)</f>
@@ -7044,7 +7044,7 @@
       </c>
       <c r="B295">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C295">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B295),A295+1)</f>
@@ -7058,7 +7058,7 @@
       </c>
       <c r="B296">
         <f t="shared" si="9"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C296">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B296),A296+1)</f>
@@ -7072,7 +7072,7 @@
       </c>
       <c r="B297">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C297">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B297),A297+1)</f>
@@ -7086,7 +7086,7 @@
       </c>
       <c r="B298">
         <f t="shared" si="9"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C298">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B298),A298+1)</f>
@@ -7100,7 +7100,7 @@
       </c>
       <c r="B299">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C299">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B299),A299+1)</f>
@@ -7114,7 +7114,7 @@
       </c>
       <c r="B300">
         <f t="shared" si="9"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C300">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B300),A300+1)</f>
@@ -7128,7 +7128,7 @@
       </c>
       <c r="B301">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C301">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B301),A301+1)</f>
@@ -7146,7 +7146,7 @@
       </c>
       <c r="C302">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B302),A302+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.15">
@@ -7342,7 +7342,7 @@
       </c>
       <c r="C316">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B316),A316+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.15">
@@ -7352,7 +7352,7 @@
       </c>
       <c r="B317">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C317">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B317),A317+1)</f>
@@ -7366,7 +7366,7 @@
       </c>
       <c r="B318">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C318">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B318),A318+1)</f>
@@ -7380,7 +7380,7 @@
       </c>
       <c r="B319">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C319">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B319),A319+1)</f>
@@ -7394,7 +7394,7 @@
       </c>
       <c r="B320">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C320">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B320),A320+1)</f>
@@ -7408,11 +7408,11 @@
       </c>
       <c r="B321">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C321">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B321),A321+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.15">
@@ -7422,11 +7422,11 @@
       </c>
       <c r="B322">
         <f t="shared" ref="B322:B385" si="11">MOD(ROW()-2,$F$8)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C322">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B322),A322+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.15">
@@ -7436,7 +7436,7 @@
       </c>
       <c r="B323">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C323">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B323),A323+1)</f>
@@ -7450,7 +7450,7 @@
       </c>
       <c r="B324">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C324">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B324),A324+1)</f>
@@ -7464,7 +7464,7 @@
       </c>
       <c r="B325">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C325">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B325),A325+1)</f>
@@ -7478,7 +7478,7 @@
       </c>
       <c r="B326">
         <f t="shared" si="11"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C326">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B326),A326+1)</f>
@@ -7492,7 +7492,7 @@
       </c>
       <c r="B327">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C327">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B327),A327+1)</f>
@@ -7506,7 +7506,7 @@
       </c>
       <c r="B328">
         <f t="shared" si="11"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C328">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B328),A328+1)</f>
@@ -7520,7 +7520,7 @@
       </c>
       <c r="B329">
         <f t="shared" si="11"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C329">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B329),A329+1)</f>
@@ -7534,7 +7534,7 @@
       </c>
       <c r="B330">
         <f t="shared" si="11"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C330">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B330),A330+1)</f>
@@ -7548,11 +7548,11 @@
       </c>
       <c r="B331">
         <f t="shared" si="11"/>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C331">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B331),A331+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.15">
@@ -7562,7 +7562,7 @@
       </c>
       <c r="B332">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C332">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B332),A332+1)</f>
@@ -7576,7 +7576,7 @@
       </c>
       <c r="B333">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C333">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B333),A333+1)</f>
@@ -7590,7 +7590,7 @@
       </c>
       <c r="B334">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C334">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B334),A334+1)</f>
@@ -7604,7 +7604,7 @@
       </c>
       <c r="B335">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C335">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B335),A335+1)</f>
@@ -7618,7 +7618,7 @@
       </c>
       <c r="B336">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C336">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B336),A336+1)</f>
@@ -7632,7 +7632,7 @@
       </c>
       <c r="B337">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C337">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B337),A337+1)</f>
@@ -7646,7 +7646,7 @@
       </c>
       <c r="B338">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C338">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B338),A338+1)</f>
@@ -7660,7 +7660,7 @@
       </c>
       <c r="B339">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C339">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B339),A339+1)</f>
@@ -7674,7 +7674,7 @@
       </c>
       <c r="B340">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C340">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B340),A340+1)</f>
@@ -7688,11 +7688,11 @@
       </c>
       <c r="B341">
         <f t="shared" si="11"/>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C341">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B341),A341+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.15">
@@ -7702,11 +7702,11 @@
       </c>
       <c r="B342">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C342">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B342),A342+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.15">
@@ -7716,7 +7716,7 @@
       </c>
       <c r="B343">
         <f t="shared" si="11"/>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C343">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B343),A343+1)</f>
@@ -7730,7 +7730,7 @@
       </c>
       <c r="B344">
         <f t="shared" si="11"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C344">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B344),A344+1)</f>
@@ -7744,7 +7744,7 @@
       </c>
       <c r="B345">
         <f t="shared" si="11"/>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C345">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B345),A345+1)</f>
@@ -7758,11 +7758,11 @@
       </c>
       <c r="B346">
         <f t="shared" si="11"/>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C346">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B346),A346+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.15">
@@ -7772,7 +7772,7 @@
       </c>
       <c r="B347">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C347">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B347),A347+1)</f>
@@ -7786,7 +7786,7 @@
       </c>
       <c r="B348">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C348">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B348),A348+1)</f>
@@ -7800,7 +7800,7 @@
       </c>
       <c r="B349">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C349">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B349),A349+1)</f>
@@ -7814,7 +7814,7 @@
       </c>
       <c r="B350">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C350">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B350),A350+1)</f>
@@ -7828,7 +7828,7 @@
       </c>
       <c r="B351">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C351">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B351),A351+1)</f>
@@ -7842,7 +7842,7 @@
       </c>
       <c r="B352">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C352">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B352),A352+1)</f>
@@ -7856,7 +7856,7 @@
       </c>
       <c r="B353">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C353">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B353),A353+1)</f>
@@ -7870,7 +7870,7 @@
       </c>
       <c r="B354">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C354">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B354),A354+1)</f>
@@ -7884,7 +7884,7 @@
       </c>
       <c r="B355">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C355">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B355),A355+1)</f>
@@ -7898,7 +7898,7 @@
       </c>
       <c r="B356">
         <f t="shared" si="11"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C356">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B356),A356+1)</f>
@@ -7912,7 +7912,7 @@
       </c>
       <c r="B357">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C357">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B357),A357+1)</f>
@@ -7926,7 +7926,7 @@
       </c>
       <c r="B358">
         <f t="shared" si="11"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C358">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B358),A358+1)</f>
@@ -7940,7 +7940,7 @@
       </c>
       <c r="B359">
         <f t="shared" si="11"/>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C359">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B359),A359+1)</f>
@@ -7954,7 +7954,7 @@
       </c>
       <c r="B360">
         <f t="shared" si="11"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C360">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B360),A360+1)</f>
@@ -7968,7 +7968,7 @@
       </c>
       <c r="B361">
         <f t="shared" si="11"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C361">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B361),A361+1)</f>
@@ -7986,7 +7986,7 @@
       </c>
       <c r="C362">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B362),A362+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.15">
@@ -8182,7 +8182,7 @@
       </c>
       <c r="C376">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B376),A376+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.15">
@@ -8192,7 +8192,7 @@
       </c>
       <c r="B377">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C377">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B377),A377+1)</f>
@@ -8206,7 +8206,7 @@
       </c>
       <c r="B378">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C378">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B378),A378+1)</f>
@@ -8220,7 +8220,7 @@
       </c>
       <c r="B379">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C379">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B379),A379+1)</f>
@@ -8234,7 +8234,7 @@
       </c>
       <c r="B380">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C380">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B380),A380+1)</f>
@@ -8248,11 +8248,11 @@
       </c>
       <c r="B381">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C381">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B381),A381+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.15">
@@ -8262,7 +8262,7 @@
       </c>
       <c r="B382">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C382">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B382),A382+1)</f>
@@ -8276,7 +8276,7 @@
       </c>
       <c r="B383">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C383">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B383),A383+1)</f>
@@ -8290,7 +8290,7 @@
       </c>
       <c r="B384">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C384">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B384),A384+1)</f>
@@ -8304,7 +8304,7 @@
       </c>
       <c r="B385">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C385">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B385),A385+1)</f>
@@ -8318,7 +8318,7 @@
       </c>
       <c r="B386">
         <f t="shared" ref="B386:B401" si="13">MOD(ROW()-2,$F$8)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C386">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B386),A386+1)</f>
@@ -8332,7 +8332,7 @@
       </c>
       <c r="B387">
         <f t="shared" si="13"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C387">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B387),A387+1)</f>
@@ -8346,7 +8346,7 @@
       </c>
       <c r="B388">
         <f t="shared" si="13"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C388">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B388),A388+1)</f>
@@ -8360,7 +8360,7 @@
       </c>
       <c r="B389">
         <f t="shared" si="13"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C389">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B389),A389+1)</f>
@@ -8374,7 +8374,7 @@
       </c>
       <c r="B390">
         <f t="shared" si="13"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C390">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B390),A390+1)</f>
@@ -8388,7 +8388,7 @@
       </c>
       <c r="B391">
         <f t="shared" si="13"/>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C391">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B391),A391+1)</f>
@@ -8402,7 +8402,7 @@
       </c>
       <c r="B392">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C392">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B392),A392+1)</f>
@@ -8416,7 +8416,7 @@
       </c>
       <c r="B393">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C393">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B393),A393+1)</f>
@@ -8430,7 +8430,7 @@
       </c>
       <c r="B394">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C394">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B394),A394+1)</f>
@@ -8444,7 +8444,7 @@
       </c>
       <c r="B395">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C395">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B395),A395+1)</f>
@@ -8458,7 +8458,7 @@
       </c>
       <c r="B396">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C396">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B396),A396+1)</f>
@@ -8472,7 +8472,7 @@
       </c>
       <c r="B397">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C397">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B397),A397+1)</f>
@@ -8486,7 +8486,7 @@
       </c>
       <c r="B398">
         <f t="shared" si="13"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C398">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B398),A398+1)</f>
@@ -8500,7 +8500,7 @@
       </c>
       <c r="B399">
         <f t="shared" si="13"/>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C399">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B399),A399+1)</f>
@@ -8514,7 +8514,7 @@
       </c>
       <c r="B400">
         <f t="shared" si="13"/>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C400">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B400),A400+1)</f>
@@ -8528,7 +8528,7 @@
       </c>
       <c r="B401">
         <f t="shared" si="13"/>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C401">
         <f>INDEX('map source data'!$A$1:$T$20,$F$8-(B401),A401+1)</f>

</xml_diff>

<commit_message>
checkpoint not moving. checkpoint2 not found.
</commit_message>
<xml_diff>
--- a/BlockTileSystem/Assets/Levels/map_schema.xlsx
+++ b/BlockTileSystem/Assets/Levels/map_schema.xlsx
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -380,18 +380,6 @@
   </si>
   <si>
     <t>East</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -730,8 +718,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="表20" displayName="表20" ref="M1:S5" tableType="xml" totalsRowShown="0" connectionId="8">
-  <autoFilter ref="M1:S5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="表20" displayName="表20" ref="M1:S3" tableType="xml" totalsRowShown="0" connectionId="8">
+  <autoFilter ref="M1:S3"/>
   <tableColumns count="7">
     <tableColumn id="1" uniqueName="x" name="vPositionX">
       <xmlColumnPr mapId="10" xpath="/SavableLevel/pPushers/PusherInXML/vPosition/x" xmlDataType="integer"/>
@@ -865,8 +853,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="表16" displayName="表16" ref="AV1:AY4" tableType="xml" totalsRowShown="0" connectionId="8">
-  <autoFilter ref="AV1:AY4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="表16" displayName="表16" ref="AV1:AY3" tableType="xml" totalsRowShown="0" connectionId="8">
+  <autoFilter ref="AV1:AY3"/>
   <tableColumns count="4">
     <tableColumn id="1" uniqueName="x" name="vCheckPoint1PositionX">
       <xmlColumnPr mapId="10" xpath="/SavableLevel/cCheckPoints/CheckPointInXML/vCheckPoint1Position/x" xmlDataType="integer"/>
@@ -2476,8 +2464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.75" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2905,27 +2893,13 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="M4" s="1">
-        <v>7</v>
-      </c>
-      <c r="N4" s="1">
-        <v>7</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>4</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="S4" s="1">
-        <v>0.8</v>
-      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
       <c r="AU4" t="s">
         <v>44</v>
       </c>
@@ -2949,27 +2923,13 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="M5" s="1">
-        <v>8</v>
-      </c>
-      <c r="N5" s="1">
-        <v>8</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>4</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="S5" s="1">
-        <v>0.8</v>
-      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:51" x14ac:dyDescent="0.15">
       <c r="A6">

</xml_diff>